<commit_message>
Removed EN for APD5052 Out4
</commit_message>
<xml_diff>
--- a/hardware/altium/Project Outputs for atfc/BOM.xlsx
+++ b/hardware/altium/Project Outputs for atfc/BOM.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="351">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="350">
   <si>
     <t>Comment</t>
   </si>
@@ -153,9 +153,6 @@
   </si>
   <si>
     <t>Polarized Capacitor (Surface Mount)</t>
-  </si>
-  <si>
-    <t>C88</t>
   </si>
   <si>
     <t>C7343</t>
@@ -1500,13 +1497,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="M57" sqref="M57"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" width="15.42578125" customWidth="1"/>
+    <col min="1" max="2" width="15.42578125" customWidth="1"/>
+    <col min="3" max="3" width="107" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="15.42578125" customWidth="1"/>
     <col min="7" max="7" width="15.5703125" customWidth="1"/>
     <col min="8" max="8" width="9.140625" style="8"/>
     <col min="10" max="10" width="16" bestFit="1" customWidth="1"/>
@@ -1536,16 +1535,16 @@
         <v>6</v>
       </c>
       <c r="H1" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>260</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>261</v>
       </c>
-      <c r="J1" s="4" t="s">
+      <c r="K1" s="4" t="s">
         <v>262</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
@@ -1579,7 +1578,7 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>12</v>
@@ -1608,13 +1607,13 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>16</v>
@@ -1637,7 +1636,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>12</v>
@@ -1666,7 +1665,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>12</v>
@@ -1695,7 +1694,7 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>12</v>
@@ -1724,7 +1723,7 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>12</v>
@@ -1753,7 +1752,7 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>12</v>
@@ -1782,13 +1781,13 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>25</v>
@@ -1811,13 +1810,13 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>16</v>
@@ -1867,7 +1866,7 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>12</v>
@@ -1925,7 +1924,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>12</v>
@@ -1960,38 +1959,38 @@
         <v>42</v>
       </c>
       <c r="C16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="3">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="F16" s="3">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="H16" s="6">
         <v>1793874</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="K16" s="2"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>14</v>
@@ -2014,13 +2013,13 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>14</v>
@@ -2032,7 +2031,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H18" s="6">
         <v>2494232</v>
@@ -2043,13 +2042,13 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>14</v>
@@ -2072,13 +2071,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>14</v>
@@ -2101,13 +2100,13 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>16</v>
@@ -2119,7 +2118,7 @@
         <v>2</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="H21" s="6">
         <v>2627389</v>
@@ -2130,13 +2129,13 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>14</v>
@@ -2159,13 +2158,13 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>16</v>
@@ -2177,7 +2176,7 @@
         <v>1</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H23" s="6">
         <v>2627368</v>
@@ -2188,13 +2187,13 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>12</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>16</v>
@@ -2206,7 +2205,7 @@
         <v>1</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H24" s="6">
         <v>1758912</v>
@@ -2217,25 +2216,25 @@
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>42</v>
       </c>
       <c r="C25" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="E25" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="F25" s="3">
         <v>4</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H25" s="6">
         <v>197038</v>
@@ -2246,19 +2245,19 @@
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="E26" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="F26" s="3">
         <v>5</v>
@@ -2275,19 +2274,19 @@
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="D27" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E27" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="F27" s="3">
         <v>2</v>
@@ -2304,19 +2303,19 @@
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C28" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D28" s="2" t="s">
-        <v>71</v>
-      </c>
       <c r="E28" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F28" s="3">
         <v>1</v>
@@ -2333,19 +2332,19 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="D29" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="E29" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="E29" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="F29" s="3">
         <v>1</v>
@@ -2356,25 +2355,25 @@
       <c r="H29" s="6"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K29" s="2"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>78</v>
-      </c>
       <c r="D30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E30" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="F30" s="3">
         <v>1</v>
@@ -2385,25 +2384,25 @@
       <c r="H30" s="6"/>
       <c r="I30" s="2"/>
       <c r="J30" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="K30" s="2"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="C31" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="D31" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F31" s="3">
         <v>1</v>
@@ -2420,19 +2419,19 @@
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="C32" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="D32" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="F32" s="3">
         <v>1</v>
@@ -2449,19 +2448,19 @@
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C33" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D33" s="2" t="s">
+      <c r="E33" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>90</v>
       </c>
       <c r="F33" s="3">
         <v>2</v>
@@ -2478,25 +2477,25 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="C34" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C34" s="2" t="s">
+      <c r="D34" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="E34" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F34" s="3">
+        <v>1</v>
+      </c>
+      <c r="G34" s="2" t="s">
         <v>94</v>
-      </c>
-      <c r="E34" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F34" s="3">
-        <v>1</v>
-      </c>
-      <c r="G34" s="2" t="s">
-        <v>95</v>
       </c>
       <c r="H34" s="6">
         <v>2288281</v>
@@ -2507,25 +2506,25 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="B35" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C35" s="2" t="s">
+      <c r="D35" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F35" s="3">
+        <v>1</v>
+      </c>
+      <c r="G35" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E35" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F35" s="3">
-        <v>1</v>
-      </c>
-      <c r="G35" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="H35" s="6">
         <v>2288277</v>
@@ -2536,25 +2535,25 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C36" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="B36" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C36" s="2" t="s">
+      <c r="D36" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F36" s="3">
+        <v>1</v>
+      </c>
+      <c r="G36" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F36" s="3">
-        <v>1</v>
-      </c>
-      <c r="G36" s="2" t="s">
-        <v>101</v>
       </c>
       <c r="H36" s="6">
         <v>2288282</v>
@@ -2565,25 +2564,25 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C37" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C37" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>104</v>
-      </c>
       <c r="E37" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F37" s="3">
         <v>1</v>
       </c>
       <c r="G37" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H37" s="6">
         <v>2457559</v>
@@ -2594,25 +2593,25 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F38" s="3">
         <v>4</v>
       </c>
       <c r="G38" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H38" s="6">
         <v>2352662</v>
@@ -2623,19 +2622,19 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>305</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>306</v>
-      </c>
-      <c r="D39" s="2" t="s">
+      <c r="E39" s="2" t="s">
         <v>107</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>108</v>
       </c>
       <c r="F39" s="3">
         <v>2</v>
@@ -2652,19 +2651,19 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C40" s="2" t="s">
+      <c r="D40" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E40" s="2" t="s">
         <v>111</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>112</v>
       </c>
       <c r="F40" s="3">
         <v>1</v>
@@ -2676,28 +2675,28 @@
         <v>7472285</v>
       </c>
       <c r="I40" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="J40" s="2" t="s">
         <v>276</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>277</v>
       </c>
       <c r="K40" s="2"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B41" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C41" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C41" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="D41" s="2" t="s">
+      <c r="E41" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="F41" s="3">
         <v>2</v>
@@ -2714,19 +2713,19 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C42" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="D42" s="2" t="s">
+      <c r="E42" s="2" t="s">
         <v>118</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>119</v>
       </c>
       <c r="F42" s="3">
         <v>1</v>
@@ -2743,19 +2742,19 @@
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C43" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="D43" s="2" t="s">
+      <c r="E43" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="E43" s="2" t="s">
-        <v>123</v>
       </c>
       <c r="F43" s="3">
         <v>1</v>
@@ -2764,31 +2763,31 @@
         <v>8</v>
       </c>
       <c r="H43" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="I43" s="2" t="s">
         <v>273</v>
       </c>
-      <c r="I43" s="2" t="s">
+      <c r="J43" s="2" t="s">
         <v>274</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>275</v>
       </c>
       <c r="K43" s="2"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C44" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>126</v>
-      </c>
       <c r="E44" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F44" s="3">
         <v>1</v>
@@ -2798,34 +2797,34 @@
       </c>
       <c r="H44" s="6"/>
       <c r="I44" s="2" t="s">
+        <v>270</v>
+      </c>
+      <c r="J44" s="2" t="s">
         <v>271</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>272</v>
       </c>
       <c r="K44" s="2"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B45" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C45" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C45" s="2" t="s">
+      <c r="D45" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="E45" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F45" s="3">
+        <v>1</v>
+      </c>
+      <c r="G45" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="E45" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F45" s="3">
-        <v>1</v>
-      </c>
-      <c r="G45" s="2" t="s">
-        <v>131</v>
       </c>
       <c r="H45" s="6">
         <v>2447292</v>
@@ -2837,25 +2836,25 @@
     </row>
     <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F46" s="3">
         <v>4</v>
       </c>
       <c r="G46" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H46" s="6">
         <v>2447385</v>
@@ -2866,25 +2865,25 @@
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C47" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D47" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>135</v>
-      </c>
       <c r="E47" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F47" s="3">
         <v>6</v>
       </c>
       <c r="G47" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H47" s="6">
         <v>2072516</v>
@@ -2895,25 +2894,25 @@
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C48" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F48" s="3">
+        <v>1</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>137</v>
-      </c>
-      <c r="D48" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E48" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F48" s="3">
-        <v>1</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>138</v>
       </c>
       <c r="H48" s="6">
         <v>2502463</v>
@@ -2924,25 +2923,25 @@
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F49" s="3">
         <v>9</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H49" s="6">
         <v>2072515</v>
@@ -2953,25 +2952,25 @@
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F50" s="3">
         <v>1</v>
       </c>
       <c r="G50" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="H50" s="6">
         <v>2447187</v>
@@ -2982,25 +2981,25 @@
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F51" s="3">
         <v>6</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H51" s="6">
         <v>2447230</v>
@@ -3011,25 +3010,25 @@
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F52" s="3">
         <v>19</v>
       </c>
       <c r="G52" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="H52" s="6">
         <v>2072517</v>
@@ -3040,25 +3039,25 @@
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F53" s="3">
         <v>8</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H53" s="6">
         <v>2072753</v>
@@ -3069,25 +3068,25 @@
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F54" s="3">
         <v>6</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H54" s="6">
         <v>2072644</v>
@@ -3098,25 +3097,25 @@
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C55" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E55" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F55" s="3">
+        <v>1</v>
+      </c>
+      <c r="G55" s="2" t="s">
         <v>148</v>
-      </c>
-      <c r="D55" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F55" s="3">
-        <v>1</v>
-      </c>
-      <c r="G55" s="2" t="s">
-        <v>149</v>
       </c>
       <c r="H55" s="6">
         <v>2072711</v>
@@ -3127,25 +3126,25 @@
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C56" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F56" s="3">
+        <v>1</v>
+      </c>
+      <c r="G56" s="2" t="s">
         <v>150</v>
-      </c>
-      <c r="D56" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E56" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F56" s="3">
-        <v>1</v>
-      </c>
-      <c r="G56" s="2" t="s">
-        <v>151</v>
       </c>
       <c r="H56" s="6">
         <v>1358053</v>
@@ -3156,25 +3155,25 @@
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C57" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F57" s="3">
+        <v>1</v>
+      </c>
+      <c r="G57" s="2" t="s">
         <v>152</v>
-      </c>
-      <c r="D57" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E57" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F57" s="3">
-        <v>1</v>
-      </c>
-      <c r="G57" s="2" t="s">
-        <v>153</v>
       </c>
       <c r="H57" s="6">
         <v>2447112</v>
@@ -3185,25 +3184,25 @@
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="B58" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="C58" s="2" t="s">
+      <c r="D58" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="E58" s="2" t="s">
         <v>156</v>
-      </c>
-      <c r="E58" s="2" t="s">
-        <v>157</v>
       </c>
       <c r="F58" s="3">
         <v>3</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H58" s="6">
         <v>2079438</v>
@@ -3214,25 +3213,25 @@
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D59" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F59" s="3">
         <v>3</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="H59" s="6">
         <v>2447114</v>
@@ -3243,25 +3242,25 @@
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C60" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F60" s="3">
+        <v>1</v>
+      </c>
+      <c r="G60" s="2" t="s">
         <v>161</v>
-      </c>
-      <c r="D60" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E60" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F60" s="3">
-        <v>1</v>
-      </c>
-      <c r="G60" s="2" t="s">
-        <v>162</v>
       </c>
       <c r="H60" s="6">
         <v>2072929</v>
@@ -3272,25 +3271,25 @@
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F61" s="3">
         <v>2</v>
       </c>
       <c r="G61" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="H61" s="6">
         <v>2072526</v>
@@ -3301,25 +3300,25 @@
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F62" s="3">
         <v>2</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="H62" s="6">
         <v>2072591</v>
@@ -3330,25 +3329,25 @@
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C63" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="D63" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E63" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F63" s="3">
+        <v>1</v>
+      </c>
+      <c r="G63" s="2" t="s">
         <v>167</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F63" s="3">
-        <v>1</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>168</v>
       </c>
       <c r="H63" s="6">
         <v>2072916</v>
@@ -3359,25 +3358,25 @@
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C64" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="D64" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F64" s="3">
+        <v>1</v>
+      </c>
+      <c r="G64" s="2" t="s">
         <v>169</v>
-      </c>
-      <c r="D64" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E64" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F64" s="3">
-        <v>1</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>170</v>
       </c>
       <c r="H64" s="6">
         <v>2073255</v>
@@ -3388,25 +3387,25 @@
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C65" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F65" s="3">
+        <v>1</v>
+      </c>
+      <c r="G65" s="2" t="s">
         <v>171</v>
-      </c>
-      <c r="D65" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E65" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F65" s="3">
-        <v>1</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>172</v>
       </c>
       <c r="H65" s="6">
         <v>2074139</v>
@@ -3417,25 +3416,25 @@
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D66" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F66" s="3">
         <v>2</v>
       </c>
       <c r="G66" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H66" s="6">
         <v>2073152</v>
@@ -3446,25 +3445,25 @@
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C67" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E67" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F67" s="3">
+        <v>1</v>
+      </c>
+      <c r="G67" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F67" s="3">
-        <v>1</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="H67" s="6">
         <v>1358082</v>
@@ -3475,25 +3474,25 @@
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F68" s="3">
         <v>2</v>
       </c>
       <c r="G68" s="2" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="H68" s="6">
         <v>2072753</v>
@@ -3504,25 +3503,25 @@
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C69" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E69" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F69" s="3">
+        <v>1</v>
+      </c>
+      <c r="G69" s="2" t="s">
         <v>179</v>
-      </c>
-      <c r="D69" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E69" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F69" s="3">
-        <v>1</v>
-      </c>
-      <c r="G69" s="2" t="s">
-        <v>180</v>
       </c>
       <c r="H69" s="6">
         <v>2072872</v>
@@ -3533,25 +3532,25 @@
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C70" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E70" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F70" s="3">
+        <v>1</v>
+      </c>
+      <c r="G70" s="2" t="s">
         <v>181</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E70" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F70" s="3">
-        <v>1</v>
-      </c>
-      <c r="G70" s="2" t="s">
-        <v>182</v>
       </c>
       <c r="H70" s="6">
         <v>2073038</v>
@@ -3562,25 +3561,25 @@
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C71" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E71" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F71" s="3">
+        <v>1</v>
+      </c>
+      <c r="G71" s="2" t="s">
         <v>183</v>
-      </c>
-      <c r="D71" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E71" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F71" s="3">
-        <v>1</v>
-      </c>
-      <c r="G71" s="2" t="s">
-        <v>184</v>
       </c>
       <c r="H71" s="6">
         <v>2072752</v>
@@ -3591,25 +3590,25 @@
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C72" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D72" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E72" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F72" s="3">
+        <v>1</v>
+      </c>
+      <c r="G72" s="2" t="s">
         <v>185</v>
-      </c>
-      <c r="D72" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E72" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F72" s="3">
-        <v>1</v>
-      </c>
-      <c r="G72" s="2" t="s">
-        <v>186</v>
       </c>
       <c r="H72" s="6">
         <v>2072872</v>
@@ -3620,19 +3619,19 @@
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F73" s="3">
         <v>16</v>
@@ -3642,32 +3641,32 @@
       </c>
       <c r="H73" s="6"/>
       <c r="I73" s="2" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="J73" s="2"/>
       <c r="K73" s="2"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C74" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="E74" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F74" s="3">
+        <v>1</v>
+      </c>
+      <c r="G74" s="2" t="s">
         <v>188</v>
-      </c>
-      <c r="D74" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="E74" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F74" s="3">
-        <v>1</v>
-      </c>
-      <c r="G74" s="2" t="s">
-        <v>189</v>
       </c>
       <c r="H74" s="6">
         <v>2447354</v>
@@ -3678,25 +3677,25 @@
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C75" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="D75" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E75" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F75" s="3">
+        <v>1</v>
+      </c>
+      <c r="G75" s="2" t="s">
         <v>190</v>
-      </c>
-      <c r="D75" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E75" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F75" s="3">
-        <v>1</v>
-      </c>
-      <c r="G75" s="2" t="s">
-        <v>191</v>
       </c>
       <c r="H75" s="6">
         <v>2073087</v>
@@ -3707,25 +3706,25 @@
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D76" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F76" s="3">
         <v>1</v>
       </c>
       <c r="G76" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H76" s="6">
         <v>2447256</v>
@@ -3736,25 +3735,25 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D77" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F77" s="3">
         <v>6</v>
       </c>
       <c r="G77" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H77" s="6">
         <v>2447376</v>
@@ -3765,25 +3764,25 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F78" s="3">
         <v>2</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H78" s="6">
         <v>2447272</v>
@@ -3794,25 +3793,25 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F79" s="3">
         <v>1</v>
       </c>
       <c r="G79" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H79" s="6">
         <v>2073065</v>
@@ -3823,25 +3822,25 @@
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C80" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D80" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F80" s="3">
+        <v>1</v>
+      </c>
+      <c r="G80" s="2" t="s">
         <v>197</v>
-      </c>
-      <c r="D80" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E80" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F80" s="3">
-        <v>1</v>
-      </c>
-      <c r="G80" s="2" t="s">
-        <v>198</v>
       </c>
       <c r="H80" s="6">
         <v>2670453</v>
@@ -3852,25 +3851,25 @@
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C81" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D81" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E81" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F81" s="3">
+        <v>1</v>
+      </c>
+      <c r="G81" s="2" t="s">
         <v>199</v>
-      </c>
-      <c r="D81" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E81" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F81" s="3">
-        <v>1</v>
-      </c>
-      <c r="G81" s="2" t="s">
-        <v>200</v>
       </c>
       <c r="H81" s="6">
         <v>2073196</v>
@@ -3881,25 +3880,25 @@
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C82" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D82" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F82" s="3">
+        <v>1</v>
+      </c>
+      <c r="G82" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="D82" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E82" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F82" s="3">
-        <v>1</v>
-      </c>
-      <c r="G82" s="2" t="s">
-        <v>202</v>
       </c>
       <c r="H82" s="6">
         <v>2072769</v>
@@ -3910,25 +3909,25 @@
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C83" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F83" s="3">
+        <v>1</v>
+      </c>
+      <c r="G83" s="2" t="s">
         <v>203</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E83" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F83" s="3">
-        <v>1</v>
-      </c>
-      <c r="G83" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="H83" s="6">
         <v>1469700</v>
@@ -3939,25 +3938,25 @@
     </row>
     <row r="84" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F84" s="3">
         <v>2</v>
       </c>
       <c r="G84" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="H84" s="6">
         <v>2447183</v>
@@ -3968,25 +3967,25 @@
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C85" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="F85" s="3">
+        <v>1</v>
+      </c>
+      <c r="G85" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E85" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="F85" s="3">
-        <v>1</v>
-      </c>
-      <c r="G85" s="2" t="s">
-        <v>208</v>
       </c>
       <c r="H85" s="6">
         <v>2073119</v>
@@ -3997,19 +3996,19 @@
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D86" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="B86" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>259</v>
-      </c>
       <c r="E86" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="F86" s="3">
         <v>1</v>
@@ -4026,19 +4025,19 @@
     </row>
     <row r="87" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C87" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D87" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="D87" s="2" t="s">
+      <c r="E87" s="2" t="s">
         <v>214</v>
-      </c>
-      <c r="E87" s="2" t="s">
-        <v>215</v>
       </c>
       <c r="F87" s="3">
         <v>1</v>
@@ -4055,19 +4054,19 @@
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="B88" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="C88" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="D88" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="E88" s="2" t="s">
         <v>218</v>
-      </c>
-      <c r="D88" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="E88" s="2" t="s">
-        <v>219</v>
       </c>
       <c r="F88" s="3">
         <v>1</v>
@@ -4084,19 +4083,19 @@
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C89" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D89" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="D89" s="2" t="s">
-        <v>222</v>
-      </c>
       <c r="E89" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="F89" s="3">
         <v>1</v>
@@ -4113,19 +4112,19 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B90" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="B90" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="C90" s="2" t="s">
+      <c r="D90" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="D90" s="2" t="s">
-        <v>226</v>
-      </c>
       <c r="E90" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F90" s="3">
         <v>1</v>
@@ -4137,24 +4136,24 @@
       <c r="I90" s="2"/>
       <c r="J90" s="2"/>
       <c r="K90" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>8</v>
       </c>
       <c r="C91" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D91" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D91" s="2" t="s">
-        <v>229</v>
-      </c>
       <c r="E91" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F91" s="3">
         <v>5</v>
@@ -4163,7 +4162,7 @@
         <v>8</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
@@ -4171,19 +4170,19 @@
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="B92" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="B92" s="2" t="s">
+      <c r="C92" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="C92" s="2" t="s">
+      <c r="D92" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="D92" s="2" t="s">
-        <v>233</v>
-      </c>
       <c r="E92" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F92" s="3">
         <v>1</v>
@@ -4200,19 +4199,19 @@
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="B93" s="2" t="s">
+      <c r="C93" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="C93" s="2" t="s">
+      <c r="D93" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="D93" s="2" t="s">
+      <c r="E93" s="2" t="s">
         <v>237</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>238</v>
       </c>
       <c r="F93" s="3">
         <v>1</v>
@@ -4229,19 +4228,19 @@
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="B94" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="B94" s="2" t="s">
+      <c r="C94" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="C94" s="2" t="s">
+      <c r="D94" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="D94" s="2" t="s">
-        <v>242</v>
-      </c>
       <c r="E94" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F94" s="3">
         <v>3</v>
@@ -4258,19 +4257,19 @@
     </row>
     <row r="95" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B95" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="B95" s="2" t="s">
+      <c r="C95" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C95" s="2" t="s">
+      <c r="D95" s="2" t="s">
         <v>245</v>
       </c>
-      <c r="D95" s="2" t="s">
-        <v>246</v>
-      </c>
       <c r="E95" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F95" s="3">
         <v>2</v>
@@ -4287,19 +4286,19 @@
     </row>
     <row r="96" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="B96" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="C96" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B96" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="C96" s="2" t="s">
+      <c r="D96" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="D96" s="2" t="s">
-        <v>249</v>
-      </c>
       <c r="E96" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="F96" s="3">
         <v>1</v>
@@ -4310,25 +4309,25 @@
       <c r="H96" s="6"/>
       <c r="I96" s="2"/>
       <c r="J96" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K96" s="2"/>
     </row>
     <row r="97" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="B97" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B97" s="2" t="s">
+      <c r="C97" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="C97" s="2" t="s">
+      <c r="D97" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="D97" s="2" t="s">
-        <v>253</v>
-      </c>
       <c r="E97" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F97" s="3">
         <v>1</v>
@@ -4339,25 +4338,25 @@
       <c r="H97" s="6"/>
       <c r="I97" s="2"/>
       <c r="J97" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="K97" s="2"/>
     </row>
     <row r="98" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="B98" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="B98" s="2" t="s">
+      <c r="C98" s="2" t="s">
         <v>255</v>
       </c>
-      <c r="C98" s="2" t="s">
+      <c r="D98" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="D98" s="2" t="s">
-        <v>257</v>
-      </c>
       <c r="E98" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="F98" s="3">
         <v>1</v>
@@ -4366,17 +4365,17 @@
         <v>8</v>
       </c>
       <c r="H98" s="6" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="I98" s="2"/>
       <c r="J98" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="K98" s="2"/>
     </row>
     <row r="100" spans="1:11" x14ac:dyDescent="0.25">
       <c r="H100" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>